<commit_message>
Adding Quicksti Testcases for more Testdata
</commit_message>
<xml_diff>
--- a/Data Files/Certpay/CertpayTestdata.xlsx
+++ b/Data Files/Certpay/CertpayTestdata.xlsx
@@ -1,20 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Sush_Certpay\Data Files\Certpay\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="5715"/>
   </bookViews>
   <sheets>
-    <sheet name="SingleBureauSingleLine" sheetId="1" r:id="rId1"/>
+    <sheet name="SingleBureauSingleLineVisa" sheetId="1" r:id="rId1"/>
     <sheet name="SingleBureauMultiLine" sheetId="2" r:id="rId2"/>
     <sheet name="MultiBureauMultiLine" sheetId="3" r:id="rId3"/>
     <sheet name="MultiBureauSingleLine" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="124519"/>
-  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -22,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="57">
   <si>
     <t>FirstName</t>
   </si>
@@ -190,13 +195,16 @@
   </si>
   <si>
     <t>10.00</t>
+  </si>
+  <si>
+    <t>4716428411725021</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -242,12 +250,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -521,25 +530,25 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.140625" bestFit="1" customWidth="1"/>
@@ -552,7 +561,7 @@
     <col min="17" max="17" width="14.7109375" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -605,15 +614,15 @@
         <v>52</v>
       </c>
     </row>
-    <row r="2" spans="1:17">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>16</v>
       </c>
       <c r="B2" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>27</v>
+      <c r="C2" s="5" t="s">
+        <v>56</v>
       </c>
       <c r="D2" t="s">
         <v>18</v>
@@ -658,7 +667,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="3" spans="1:17">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>16</v>
       </c>
@@ -711,7 +720,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="4" spans="1:17">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>16</v>
       </c>
@@ -764,7 +773,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="5" spans="1:17">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>16</v>
       </c>
@@ -830,14 +839,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P5"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection sqref="A1:P5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="17.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19" bestFit="1" customWidth="1"/>
@@ -848,7 +857,7 @@
     <col min="16" max="16" width="16.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -898,7 +907,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:16">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -948,7 +957,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:16">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>16</v>
       </c>
@@ -998,7 +1007,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="4" spans="1:16">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>16</v>
       </c>
@@ -1048,7 +1057,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:16">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>16</v>
       </c>
@@ -1110,14 +1119,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P5"/>
   <sheetViews>
     <sheetView topLeftCell="B3" workbookViewId="0">
       <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.28515625" bestFit="1" customWidth="1"/>
@@ -1130,7 +1139,7 @@
     <col min="11" max="11" width="13.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1180,7 +1189,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:16">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -1230,7 +1239,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:16">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>16</v>
       </c>
@@ -1280,7 +1289,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="4" spans="1:16">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>16</v>
       </c>
@@ -1330,7 +1339,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:16">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>16</v>
       </c>
@@ -1392,16 +1401,16 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:16">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1451,7 +1460,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:16">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -1501,7 +1510,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:16">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>50</v>
       </c>
@@ -1551,7 +1560,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="4" spans="1:16">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>16</v>
       </c>
@@ -1601,7 +1610,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:16">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>16</v>
       </c>

</xml_diff>